<commit_message>
v2.2 update according to new comments
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_USERHOME.xlsx
+++ b/LH_TESTCASES/LH_TC_USERHOME.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
   <si>
     <t>Preconditions</t>
   </si>
@@ -173,10 +173,6 @@
     <t>1. User Navigates the browser url.
 2. Login with valid email and password
 3. Navigates to the [UserHome]</t>
-  </si>
-  <si>
-    <t>E-mail: user1@example.com
-Password: CorrectPassword123</t>
   </si>
   <si>
     <t>LH-TC-USERHOME-006</t>
@@ -240,6 +236,16 @@
   </si>
   <si>
     <t>v2.1</t>
+  </si>
+  <si>
+    <t>E-mail: user1@example.com
+Password: CorrectPassword@123</t>
+  </si>
+  <si>
+    <t>v2.2</t>
+  </si>
+  <si>
+    <t>update according to new comments</t>
   </si>
 </sst>
 </file>
@@ -339,7 +345,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -400,15 +406,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color theme="0"/>
       </left>
@@ -441,7 +438,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -461,7 +458,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -470,7 +466,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -485,26 +481,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -513,17 +491,35 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
@@ -932,8 +928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView zoomScale="32" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="D16" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -943,10 +939,10 @@
     <col min="3" max="3" width="110.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="86.42578125" style="1" customWidth="1"/>
     <col min="5" max="5" width="74.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="17" customWidth="1"/>
+    <col min="6" max="6" width="41.42578125" style="16" customWidth="1"/>
     <col min="7" max="7" width="142.5703125" style="1" customWidth="1"/>
     <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="14"/>
+    <col min="9" max="9" width="25.7109375" style="13"/>
     <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="21.140625" style="1" customWidth="1"/>
     <col min="12" max="16384" width="9.140625" style="1"/>
@@ -956,42 +952,42 @@
       <c r="A1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="B1" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="21"/>
-      <c r="D1" s="22"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="29"/>
+      <c r="F1" s="15"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="23" t="s">
+      <c r="B2" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="24"/>
-      <c r="D2" s="25"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="32"/>
       <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="30"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
       <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="24"/>
-      <c r="D4" s="25"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
       <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1022,7 +1018,7 @@
       <c r="F8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="13" t="s">
+      <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="7" t="s">
@@ -1035,271 +1031,271 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="12" customFormat="1" ht="188.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:10" s="11" customFormat="1" ht="188.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="31" t="s">
+      <c r="B9" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="31" t="s">
+      <c r="C9" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="31" t="s">
+      <c r="D9" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="30" t="s">
+      <c r="F9" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" s="23"/>
+      <c r="I9" s="23"/>
+      <c r="J9" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.35">
+      <c r="A10" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E10" s="21" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="H10" s="20"/>
+      <c r="I10" s="20"/>
+      <c r="J10" s="20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.35">
+      <c r="A11" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="B11" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D11" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="H11" s="23"/>
+      <c r="I11" s="23"/>
+      <c r="J11" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="25"/>
+      <c r="B12" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G12" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="H12" s="23"/>
+      <c r="I12" s="23"/>
+      <c r="J12" s="23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="25"/>
+      <c r="B13" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>52</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G13" s="22" t="s">
+        <v>61</v>
+      </c>
+      <c r="H13" s="23"/>
+      <c r="I13" s="23"/>
+      <c r="J13" s="23" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="G9" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31" t="s">
+      <c r="C14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E14" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F14" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="20"/>
+      <c r="I14" s="20"/>
+      <c r="J14" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="26"/>
+      <c r="B15" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D15" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G15" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20"/>
+      <c r="J15" s="20" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.35">
+      <c r="A16" s="26"/>
+      <c r="B16" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E16" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="G16" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="20" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.35">
-      <c r="A10" s="26" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="27" t="s">
-        <v>30</v>
-      </c>
-      <c r="C10" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="D10" s="27" t="s">
+    <row r="17" spans="1:10" s="11" customFormat="1" ht="63" x14ac:dyDescent="0.35">
+      <c r="A17" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="E17" s="22" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G10" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
-      <c r="J10" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.35">
-      <c r="A11" s="32" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="31" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="31"/>
-      <c r="I11" s="31"/>
-      <c r="J11" s="31" t="s">
+      <c r="F17" s="22" t="s">
+        <v>65</v>
+      </c>
+      <c r="G17" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="18" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="32"/>
-      <c r="B12" s="31" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" s="31" t="s">
-        <v>51</v>
-      </c>
-      <c r="D12" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="30" t="s">
-        <v>59</v>
-      </c>
-      <c r="H12" s="31"/>
-      <c r="I12" s="31"/>
-      <c r="J12" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" s="18" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="32"/>
-      <c r="B13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="D13" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="F13" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G13" s="30" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="31"/>
-      <c r="I13" s="31"/>
-      <c r="J13" s="31" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" s="18" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="29" t="s">
-        <v>43</v>
-      </c>
-      <c r="B14" s="27" t="s">
-        <v>49</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="D14" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F14" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
-      <c r="J14" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" s="18" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
-      <c r="B15" s="27" t="s">
-        <v>50</v>
-      </c>
-      <c r="C15" s="27" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E15" s="28" t="s">
-        <v>55</v>
-      </c>
-      <c r="F15" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G15" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
-      <c r="J15" s="27" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" s="12" customFormat="1" ht="126" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
-      <c r="B16" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="C16" s="28" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="E16" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="F16" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" s="12" customFormat="1" ht="63" x14ac:dyDescent="0.35">
-      <c r="A17" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="31" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="31" t="s">
-        <v>29</v>
-      </c>
-      <c r="E17" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="F17" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="G17" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="31"/>
-      <c r="I17" s="31"/>
-      <c r="J17" s="31" t="s">
-        <v>21</v>
-      </c>
-    </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="12"/>
-      <c r="B18" s="12"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="12"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12" t="s">
+      <c r="A18" s="11"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="12"/>
-      <c r="H18" s="12"/>
-      <c r="I18" s="19"/>
-      <c r="J18" s="12"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="18"/>
+      <c r="J18" s="11"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="14" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1368,7 +1364,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1380,54 +1376,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="C1" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="9" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="33">
+      <c r="D2" s="24">
         <v>45790</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="11" t="s">
+      <c r="A3" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D3" s="33">
+      <c r="C3" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="24">
         <v>45790</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="9" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="11"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
+    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="24">
+        <v>45791</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
v2.3 Test Execution Done
</commit_message>
<xml_diff>
--- a/LH_TESTCASES/LH_TC_USERHOME.xlsx
+++ b/LH_TESTCASES/LH_TC_USERHOME.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{283AEE88-B550-4B8E-8970-0413826819B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH_TC_USERHOME" sheetId="1" r:id="rId1"/>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="81">
   <si>
     <t>Preconditions</t>
   </si>
@@ -247,12 +248,51 @@
   <si>
     <t>update according to new comments</t>
   </si>
+  <si>
+    <t>Pass</t>
+  </si>
+  <si>
+    <t>Welcome, user1 is displayed clearly at the top of the page.</t>
+  </si>
+  <si>
+    <t>Go to Categories' button exists and navigates correctly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> notifications are retrieved and displayed for followed categories</t>
+  </si>
+  <si>
+    <t>No new notifiction , no count appears on th bell icon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The notification bar is labeled "Notifications from Followed Categories" </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> posts from followed categories are listed in the home page</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no posts are listed in user home page if user not follow any categorey</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> the section title above posts is labeled "Posts from Followed Categories"</t>
+  </si>
+  <si>
+    <t>bell icon shows count of new notifications</t>
+  </si>
+  <si>
+    <t>v2.3</t>
+  </si>
+  <si>
+    <t>Omar Sherif</t>
+  </si>
+  <si>
+    <t>Test Excution Done</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -314,6 +354,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -438,63 +484,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -502,110 +514,63 @@
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF006100"/>
@@ -640,9 +605,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -680,9 +645,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -717,7 +682,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -752,7 +717,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -925,382 +890,418 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J20"/>
   <sheetViews>
-    <sheetView topLeftCell="D16" zoomScale="65" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="21" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="50.28515625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="45.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="110.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="86.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="74.42578125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="41.42578125" style="16" customWidth="1"/>
-    <col min="7" max="7" width="142.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="25.7109375" style="13"/>
-    <col min="10" max="10" width="16.85546875" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="50.33203125" style="25" customWidth="1"/>
+    <col min="2" max="2" width="45.6640625" style="23" customWidth="1"/>
+    <col min="3" max="3" width="110.44140625" style="23" customWidth="1"/>
+    <col min="4" max="4" width="86.44140625" style="23" customWidth="1"/>
+    <col min="5" max="5" width="74.44140625" style="23" customWidth="1"/>
+    <col min="6" max="6" width="41.44140625" style="24" customWidth="1"/>
+    <col min="7" max="7" width="122.77734375" style="23" customWidth="1"/>
+    <col min="8" max="8" width="67" style="23" customWidth="1"/>
+    <col min="9" max="9" width="25.6640625" style="5"/>
+    <col min="10" max="10" width="16.88671875" style="23" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" style="23" customWidth="1"/>
+    <col min="12" max="16384" width="9.109375" style="23"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="2" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:10" s="17" customFormat="1" ht="66.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="28"/>
-      <c r="D1" s="29"/>
-      <c r="F1" s="15"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A2" s="4" t="s">
+      <c r="C1" s="15"/>
+      <c r="D1" s="16"/>
+      <c r="F1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A2" s="19" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="C2" s="31"/>
-      <c r="D2" s="32"/>
-      <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A3" s="4" t="s">
+      <c r="C2" s="21"/>
+      <c r="D2" s="22"/>
+      <c r="I2" s="23"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A3" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="31"/>
-      <c r="D3" s="32"/>
-      <c r="I3" s="1"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A4" s="4" t="s">
+      <c r="B3" s="20"/>
+      <c r="C3" s="21"/>
+      <c r="D3" s="22"/>
+      <c r="I3" s="23"/>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A4" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B4" s="30" t="s">
+      <c r="B4" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="31"/>
-      <c r="D4" s="32"/>
-      <c r="I4" s="1"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I5" s="1"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I6" s="1"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="I7" s="1"/>
-    </row>
-    <row r="8" spans="1:10" s="7" customFormat="1" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
+      <c r="I4" s="23"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I5" s="23"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I6" s="23"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="I7" s="23"/>
+    </row>
+    <row r="8" spans="1:10" s="4" customFormat="1" ht="25.8" x14ac:dyDescent="0.3">
+      <c r="A8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="7" t="s">
+      <c r="H8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="7" t="s">
+      <c r="J8" s="4" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:10" s="11" customFormat="1" ht="188.25" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="22" t="s">
+    <row r="9" spans="1:10" s="26" customFormat="1" ht="188.25" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="23" t="s">
+      <c r="D9" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="H9" s="23"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="23" t="s">
+      <c r="H9" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J9" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.35">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+      <c r="A10" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="21" t="s">
+      <c r="F10" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G10" s="21" t="s">
+      <c r="G10" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="H10" s="20"/>
-      <c r="I10" s="20"/>
-      <c r="J10" s="20" t="s">
+      <c r="H10" s="29" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J10" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:10" ht="63" x14ac:dyDescent="0.4">
+      <c r="A11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="23"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23" t="s">
+      <c r="H11" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J11" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
-      <c r="B12" s="23" t="s">
+    <row r="12" spans="1:10" s="27" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A12" s="11"/>
+      <c r="B12" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="23" t="s">
+      <c r="D12" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="H12" s="23"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23" t="s">
+      <c r="H12" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J12" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="25"/>
-      <c r="B13" s="23" t="s">
+    <row r="13" spans="1:10" s="27" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A13" s="11"/>
+      <c r="B13" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="H13" s="23"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="23" t="s">
+      <c r="H13" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J13" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:10" s="27" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="21" t="s">
+      <c r="E14" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="21" t="s">
+      <c r="F14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="20" t="s">
+      <c r="G14" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="20"/>
-      <c r="I14" s="20"/>
-      <c r="J14" s="20" t="s">
+      <c r="H14" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I14" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J14" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:10" s="17" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="26"/>
-      <c r="B15" s="20" t="s">
+    <row r="15" spans="1:10" s="27" customFormat="1" ht="166.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A15" s="12"/>
+      <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D15" s="20" t="s">
+      <c r="D15" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E15" s="21" t="s">
+      <c r="E15" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="21" t="s">
+      <c r="F15" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="20" t="s">
+      <c r="G15" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="H15" s="20"/>
-      <c r="I15" s="20"/>
-      <c r="J15" s="20" t="s">
+      <c r="H15" s="8" t="s">
+        <v>75</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J15" s="8" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="16" spans="1:10" s="11" customFormat="1" ht="126" x14ac:dyDescent="0.35">
-      <c r="A16" s="26"/>
-      <c r="B16" s="20" t="s">
+    <row r="16" spans="1:10" s="26" customFormat="1" ht="105" x14ac:dyDescent="0.4">
+      <c r="A16" s="12"/>
+      <c r="B16" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C16" s="21" t="s">
+      <c r="C16" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="20" t="s">
+      <c r="D16" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="F16" s="21" t="s">
+      <c r="F16" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="21" t="s">
+      <c r="G16" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="H16" s="20"/>
-      <c r="I16" s="20"/>
-      <c r="J16" s="20" t="s">
+      <c r="H16" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="J16" s="8" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:10" s="11" customFormat="1" ht="63" x14ac:dyDescent="0.35">
-      <c r="A17" s="22" t="s">
+    <row r="17" spans="1:10" s="26" customFormat="1" ht="63" x14ac:dyDescent="0.4">
+      <c r="A17" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B17" s="23" t="s">
+      <c r="B17" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D17" s="23" t="s">
+      <c r="D17" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="23"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="23" t="s">
+      <c r="H17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="J17" s="9" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="A18" s="11"/>
-      <c r="B18" s="11"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11" t="s">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="A18" s="26"/>
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="26"/>
+      <c r="F18" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G18" s="11"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="18"/>
-      <c r="J18" s="11"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F19" s="14" t="s">
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="26"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F19" s="28" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
-      <c r="F20" s="14" t="s">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.4">
+      <c r="F20" s="28" t="s">
         <v>19</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A8:I9"/>
+  <autoFilter ref="A8:I9" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <mergeCells count="6">
     <mergeCell ref="A11:A13"/>
     <mergeCell ref="A14:A16"/>
@@ -1309,48 +1310,16 @@
     <mergeCell ref="B3:D3"/>
     <mergeCell ref="B4:D4"/>
   </mergeCells>
-  <conditionalFormatting sqref="I9:I11 I14 I17:I1048576">
-    <cfRule type="containsText" dxfId="9" priority="9" operator="containsText" text="Fail">
+  <conditionalFormatting sqref="I9:I1048576">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
       <formula>NOT(ISERROR(SEARCH("Fail",I9)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="10" operator="containsText" text="Pass">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
       <formula>NOT(ISERROR(SEARCH("Pass",I9)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I12">
-    <cfRule type="containsText" dxfId="7" priority="7" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I12)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="8" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I12)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I15">
-    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I15)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I13">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I13)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I13)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="Fail">
-      <formula>NOT(ISERROR(SEARCH("Fail",I16)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Pass">
-      <formula>NOT(ISERROR(SEARCH("Pass",I16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I9:I1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Pass, Fail, Blocked, N/A"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1360,78 +1329,93 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="46.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="1" max="1" width="31.6640625" customWidth="1"/>
+    <col min="2" max="2" width="18.33203125" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="6" customFormat="1" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="10">
         <v>45790</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="10">
         <v>45790</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="24">
+      <c r="D4" s="10">
         <v>45791</v>
       </c>
     </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D5" s="10">
+        <v>45792</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>